<commit_message>
Version 1.3.18 - Release to PyPI
</commit_message>
<xml_diff>
--- a/TherapyNoglossNodecision.xlsx
+++ b/TherapyNoglossNodecision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/PyPI/github/pyDMNrules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{CF3451BD-2D5C-48F1-AF1F-87215C9916AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F17FE236-F606-43FD-B0BE-C9E1D0CAA5BD}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{CF3451BD-2D5C-48F1-AF1F-87215C9916AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ECCEBFB-98CE-4D09-A40E-A5C5BD8319A6}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="784" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DecisionMedication" sheetId="7" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Encounter Diagnosis</t>
   </si>
@@ -214,28 +214,16 @@
     <t>DecisionMedication</t>
   </si>
   <si>
-    <t>defMed</t>
-  </si>
-  <si>
-    <t>calcClear</t>
-  </si>
-  <si>
-    <t>defDose</t>
-  </si>
-  <si>
-    <t>warnInt</t>
-  </si>
-  <si>
     <t>error</t>
   </si>
   <si>
     <t>Execute</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>decimal((140 - Data.Patient_Age) * (Patient Weight )/ (Patient Creatinine Level * 72),6)</t>
+  </si>
+  <si>
+    <t>prescribe</t>
   </si>
 </sst>
 </file>
@@ -569,7 +557,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -791,15 +779,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -817,6 +796,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1301,91 +1283,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="9.109375" style="1"/>
     <col min="3" max="3" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.609375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="7" width="28.609375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="2:4" s="2" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="2:7" s="2" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="74" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" s="2" customFormat="1" ht="12.6" thickTop="1" x14ac:dyDescent="0.4">
+        <v>52</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="2" customFormat="1" ht="12.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B4" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="81" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="76"/>
+        <v>51</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="76"/>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C4:C7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1409,10 +1385,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="21"/>
     </row>
     <row r="3" spans="2:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1486,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1499,10 +1475,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:5" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="53" t="s">
@@ -1523,7 +1499,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="70" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" s="72" t="s">
         <v>11</v>
@@ -1563,10 +1539,10 @@
   <sheetData>
     <row r="1" spans="2:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="82"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
@@ -1656,10 +1632,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1725,10 +1701,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:4" ht="12.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
@@ -1738,7 +1714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="24.9" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" ht="12.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B4" s="57" t="s">
         <v>39</v>
       </c>

</xml_diff>